<commit_message>
create postgre.js and connect to postgre DB
</commit_message>
<xml_diff>
--- a/HC realationship_oracle.xlsx
+++ b/HC realationship_oracle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\node_HC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C09C1B35-F60A-46C7-A969-D2E3F5107225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B8506F-A468-478B-9A5D-4ED756C8ADE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="3285" windowWidth="28800" windowHeight="15435" xr2:uid="{3FEB9EA8-B38D-4ABB-BAFF-992DF5813F27}"/>
+    <workbookView xWindow="30612" yWindow="2508" windowWidth="23256" windowHeight="13176" xr2:uid="{3FEB9EA8-B38D-4ABB-BAFF-992DF5813F27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="83">
   <si>
     <t>season</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -346,6 +346,22 @@
   </si>
   <si>
     <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boardImg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board_img_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>board_img_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>admin_email</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -417,7 +433,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -477,13 +493,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -505,11 +541,23 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,10 +873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17967663-B4AF-4DD8-9D61-2A36F6DE7A44}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -853,7 +901,7 @@
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -877,11 +925,11 @@
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="8"/>
       <c r="D7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -918,14 +966,14 @@
       <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -989,8 +1037,8 @@
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
       <c r="E15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1069,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -1040,18 +1088,18 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
       <c r="E19" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>70</v>
       </c>
@@ -1068,7 +1116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1085,23 +1133,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="7"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
@@ -1139,7 +1187,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>19</v>
       </c>
@@ -1177,16 +1225,16 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -1203,7 +1251,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>19</v>
       </c>
@@ -1220,27 +1268,31 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
+    <row r="31" spans="1:13" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="3" t="s">
@@ -1255,21 +1307,33 @@
       <c r="G32" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H32" s="3" t="s">
+      <c r="H32" s="9" t="s">
         <v>40</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -1284,26 +1348,38 @@
       <c r="G33" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="H33" s="9" t="s">
         <v>67</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="J33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
       <c r="F35" s="1" t="s">
         <v>76</v>
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>43</v>
       </c>
@@ -1323,7 +1399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -1343,15 +1419,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>49</v>
       </c>
@@ -1365,7 +1441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
@@ -1379,23 +1455,26 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="8"/>
+      <c r="J43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="3" t="s">
@@ -1404,8 +1483,17 @@
       <c r="E44" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44" t="s">
+        <v>80</v>
+      </c>
+      <c r="K44" t="s">
+        <v>81</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>20</v>
       </c>
@@ -1422,21 +1510,21 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="26.25" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>47</v>
@@ -1469,9 +1557,9 @@
       <c r="A51" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="8"/>
       <c r="E51" s="3" t="s">
         <v>78</v>
       </c>
@@ -1506,21 +1594,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A43:E43"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="E19:F19"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A31:M31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>